<commit_message>
Suite registrar vuelo, falta el cp006.
</commit_message>
<xml_diff>
--- a/MercuryTours/Resources/datapool/CamposRegister.xlsx
+++ b/MercuryTours/Resources/datapool/CamposRegister.xlsx
@@ -1,24 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anamariaquinteroleal/Documents/WS_Algoritmos/MercuryTours/Resources/datapool/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="5070" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>First Name</t>
   </si>
@@ -63,6 +56,27 @@
   </si>
   <si>
     <t>User Name</t>
+  </si>
+  <si>
+    <t>Fabian</t>
+  </si>
+  <si>
+    <t>Alfonso</t>
+  </si>
+  <si>
+    <t>elkin3001</t>
+  </si>
+  <si>
+    <t>Galan M#14</t>
+  </si>
+  <si>
+    <t>Calarca</t>
+  </si>
+  <si>
+    <t>Quindio</t>
+  </si>
+  <si>
+    <t>Colombia</t>
   </si>
 </sst>
 </file>
@@ -116,6 +130,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -386,25 +403,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="7" style="2" customWidth="1"/>
     <col min="7" max="7" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="10.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,8 +461,43 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E2" s="1"/>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2">
+        <v>311</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="2">
+        <v>57</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>